<commit_message>
Fixed PID task still need to tune but will work for now
</commit_message>
<xml_diff>
--- a/X Axis Excel Doc.xlsx
+++ b/X Axis Excel Doc.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maara\Documents\.Art\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maaran\Documents\Temp School\MTE\.art\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD6FB6CE-B5F8-4911-A6C1-39518AB2FEA0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A784FACA-FA50-4C53-9DB0-805687EC5FDE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12375" xr2:uid="{E051B108-B8FF-42D4-B98A-7908CA185272}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Forwards" sheetId="1" r:id="rId1"/>
+    <sheet name="Reverse" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -89,37 +89,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -216,7 +186,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$11</c:f>
+              <c:f>Forwards!$B$1:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -258,7 +228,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$1:$C$11</c:f>
+              <c:f>Forwards!$C$1:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -266,34 +236,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>156.66</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>323.33</c:v>
+                  <c:v>32.033299999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>404.99</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>646.66</c:v>
+                  <c:v>65.332999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>811.66</c:v>
+                  <c:v>81.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>963.33</c:v>
+                  <c:v>98.165999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1113.33</c:v>
+                  <c:v>110.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1208</c:v>
+                  <c:v>125.33</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1215</c:v>
+                  <c:v>125.66</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1230</c:v>
+                  <c:v>127.07</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -633,7 +603,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$1:$C$11</c:f>
+              <c:f>Forwards!$C$1:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -641,41 +611,41 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>156.66</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>323.33</c:v>
+                  <c:v>32.033299999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>404.99</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>646.66</c:v>
+                  <c:v>65.332999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>811.66</c:v>
+                  <c:v>81.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>963.33</c:v>
+                  <c:v>98.165999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1113.33</c:v>
+                  <c:v>110.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1208</c:v>
+                  <c:v>125.33</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1215</c:v>
+                  <c:v>125.66</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1230</c:v>
+                  <c:v>127.07</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$11</c:f>
+              <c:f>Forwards!$B$1:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -909,6 +879,860 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.3381889763779521E-2"/>
+          <c:y val="0.18560185185185185"/>
+          <c:w val="0.90972922134733158"/>
+          <c:h val="0.77736111111111106"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.3888888888888893E-4"/>
+                  <c:y val="-0.15319444444444444"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Reverse!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Reverse!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-15.166</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-48.33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-64.66</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-81.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-96.66</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-111.88</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-117.33</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-121.66</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-123.33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-87CD-4E6A-8EA8-9033138E9473}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="518986640"/>
+        <c:axId val="518989264"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="518986640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="518989264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="518989264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="518986640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.3381889763779521E-2"/>
+          <c:y val="0.18560185185185185"/>
+          <c:w val="0.90972922134733158"/>
+          <c:h val="0.77736111111111106"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.3888888888888893E-4"/>
+                  <c:y val="-0.15319444444444444"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Reverse!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-15.166</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-48.33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-64.66</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-81.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-96.66</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-111.88</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-117.33</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-121.66</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-123.33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Reverse!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2180-4F59-B223-786F4E0D53BA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="518986640"/>
+        <c:axId val="518989264"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="518986640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="518989264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="518989264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="518986640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -989,6 +1813,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1506,6 +2410,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2082,6 +4018,85 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>183355</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>154781</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>221455</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>2381</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{636DB7AE-9EB1-4A4F-9160-9B5079F2AD26}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C12C7616-EF8F-47F3-8303-570463BFEAA7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2398,12 +4413,12 @@
   <dimension ref="B1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B1" sqref="B1:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B1">
         <v>0</v>
       </c>
@@ -2411,84 +4426,188 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B2">
         <v>10</v>
       </c>
       <c r="C2">
-        <v>156.66</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B3">
         <v>20</v>
       </c>
       <c r="C3">
-        <v>323.33</v>
+        <v>32.033299999999997</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B4">
         <v>30</v>
       </c>
       <c r="C4">
-        <v>404.99</v>
+        <v>48.5</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5">
         <v>40</v>
       </c>
       <c r="C5">
-        <v>646.66</v>
+        <v>65.332999999999998</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>50</v>
       </c>
       <c r="C6">
-        <v>811.66</v>
+        <v>81.5</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>60</v>
       </c>
       <c r="C7">
-        <v>963.33</v>
+        <v>98.165999999999997</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>70</v>
       </c>
       <c r="C8">
-        <v>1113.33</v>
+        <v>110.5</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>80</v>
       </c>
       <c r="C9">
-        <v>1208</v>
+        <v>125.33</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>90</v>
       </c>
       <c r="C10">
-        <v>1215</v>
+        <v>125.66</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B11">
         <v>100</v>
       </c>
       <c r="C11">
-        <v>1230</v>
+        <v>127.07</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7615254E-2D50-4B71-9A4C-D428673B485E}">
+  <dimension ref="B2:C12"/>
+  <sheetViews>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B3">
+        <v>-10</v>
+      </c>
+      <c r="C3">
+        <v>-15.166</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B4">
+        <v>-20</v>
+      </c>
+      <c r="C4">
+        <v>-33</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B5">
+        <v>-30</v>
+      </c>
+      <c r="C5">
+        <v>-48.33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B6">
+        <v>-40</v>
+      </c>
+      <c r="C6">
+        <v>-64.66</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B7">
+        <v>-50</v>
+      </c>
+      <c r="C7">
+        <v>-81.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B8">
+        <v>-60</v>
+      </c>
+      <c r="C8">
+        <v>-96.66</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B9">
+        <v>-70</v>
+      </c>
+      <c r="C9">
+        <v>-111.88</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B10">
+        <v>-80</v>
+      </c>
+      <c r="C10">
+        <v>-117.33</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B11">
+        <v>-90</v>
+      </c>
+      <c r="C11">
+        <v>-121.66</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B12">
+        <v>-100</v>
+      </c>
+      <c r="C12">
+        <v>-123.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>